<commit_message>
Adding constraints for Caesar cipher to backlog
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3610f7e960ad896b/Dokumenty/PUT/4 semester/SE/Text-Transformer-main/Text-Transformer-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3610f7e960ad896b/Dokumenty/PUT/4 semester/SE/Text-Transformer/Text-Transformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_E4BE2359C700430BC3A6B9EA214E1B09624CFD55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2767A66-A667-4B25-9287-42D651E2EECA}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_E4BE2359C700430BC3A6B9EA214E1B09624CFD55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C517313-E16C-429C-8ABE-BF20D9BBA0B2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -247,11 +247,6 @@
     <t>As a user, I can convert Roman numbers to Arabic</t>
   </si>
   <si>
-    <t>• Depending on the input, shift each letter by n places in the alphabet
-• Example for n=2: 'abc' -&gt; 'cde'
-• Example for n=3: 'abc' -&gt; 'def'</t>
-  </si>
-  <si>
     <t>• XX -&gt; 20
 • IV -&gt; 4</t>
   </si>
@@ -260,6 +255,11 @@
   </si>
   <si>
     <t>Create function romanToArabic()</t>
+  </si>
+  <si>
+    <t>• Depending on the input, shift each letter by n places in the alphabet
+• Alphabet is composed of lowercase and uppercase letters and space
+• Example for n=3: 'abc' -&gt; 'def' (input: '3abc')</t>
   </si>
 </sst>
 </file>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8799,7 +8799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -9301,7 +9301,7 @@
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="7">
         <v>2</v>
@@ -9319,7 +9319,7 @@
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="7">
         <v>2</v>

</xml_diff>

<commit_message>
Add items to backlog for sprint 2
</commit_message>
<xml_diff>
--- a/TextTransformer.xlsx
+++ b/TextTransformer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3610f7e960ad896b/Dokumenty/PUT/4 semester/SE/Text-Transformer/Text-Transformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_E4BE2359C700430BC3A6B9EA214E1B09624CFD55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E4EA7C1-9FC2-408E-8A94-71C6003ECD1E}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="11_E4BE2359C700430BC3A6B9EA214E1B09624CFD55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED26D357-3D69-4B81-BEB3-C63493119897}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>Text Transformer</t>
   </si>
@@ -260,6 +260,27 @@
     <t>• Depending on the input, shift each letter by n places in the alphabet
 • Alphabet is composed of lowercase and uppercase letters
 • Example for n=3: 'abc' -&gt; 'def' (input: '3abc')</t>
+  </si>
+  <si>
+    <t>As a user, I can view statistics about text</t>
+  </si>
+  <si>
+    <t>• Number of words
+• Numbers of characters</t>
+  </si>
+  <si>
+    <t>As a user, I can decipher text using Caesar cipher</t>
+  </si>
+  <si>
+    <t>• Depending on the input, shift each letter by -n places in the alphabet
+• Alphabet is composed of lowercase and uppercase letters
+• Example for n=3: 'def' -&gt; 'abc' (input: '3def')</t>
+  </si>
+  <si>
+    <t>Create function caesarDecipher()</t>
+  </si>
+  <si>
+    <t>Create function viewStats()</t>
   </si>
 </sst>
 </file>
@@ -1632,10 +1653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1874,18 +1895,38 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
@@ -8781,13 +8822,6 @@
       <c r="C999" s="7"/>
       <c r="D999" s="7"/>
       <c r="E999" s="6"/>
-    </row>
-    <row r="1000" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1000" s="6"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="7"/>
-      <c r="D1000" s="7"/>
-      <c r="E1000" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
@@ -8799,8 +8833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9326,24 +9360,40 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
+      <c r="A37" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
+      <c r="C37" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
+      <c r="A39" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
+      <c r="B40" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>

</xml_diff>